<commit_message>
Day - 8 init
</commit_message>
<xml_diff>
--- a/Angular-Java Plan.xlsx
+++ b/Angular-Java Plan.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t xml:space="preserve">Day </t>
   </si>
@@ -389,6 +389,9 @@
       </rPr>
       <t xml:space="preserve"> - Hooks (useState, useEffect), API handling using fakestoreapi.com</t>
     </r>
+  </si>
+  <si>
+    <t>Learnt basics of react and different components</t>
   </si>
 </sst>
 </file>
@@ -864,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -905,20 +908,20 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="88.5" customHeight="1">
-      <c r="A2" s="3">
-        <v>6</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>14</v>
+      <c r="A2" s="11">
+        <v>7</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>44</v>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -929,19 +932,19 @@
     </row>
     <row r="3" spans="1:11" ht="88.5" customHeight="1">
       <c r="A3" s="3">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -952,19 +955,19 @@
     </row>
     <row r="4" spans="1:11" ht="88.5" customHeight="1">
       <c r="A4" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>41</v>
+      <c r="E4" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -975,19 +978,19 @@
     </row>
     <row r="5" spans="1:11" ht="88.5" customHeight="1">
       <c r="A5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>40</v>
+      <c r="E5" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -998,19 +1001,19 @@
     </row>
     <row r="6" spans="1:11" ht="88.5" customHeight="1">
       <c r="A6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1021,19 +1024,19 @@
     </row>
     <row r="7" spans="1:11" ht="88.5" customHeight="1">
       <c r="A7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1042,18 +1045,22 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="91.5" customHeight="1">
-      <c r="A8" s="11">
-        <v>7</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+    <row r="8" spans="1:11" ht="88.5" customHeight="1">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1061,15 +1068,15 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="48.75" customHeight="1">
+    <row r="9" spans="1:11" ht="91.5" customHeight="1">
       <c r="A9" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>46</v>
+        <v>15</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1080,15 +1087,15 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="67.5" customHeight="1">
+    <row r="10" spans="1:11" ht="48.75" customHeight="1">
       <c r="A10" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1099,15 +1106,15 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="64.5" customHeight="1">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>20</v>
+    <row r="11" spans="1:11" ht="67.5" customHeight="1">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1118,12 +1125,12 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="67.5" customHeight="1">
+    <row r="12" spans="1:11" ht="64.5" customHeight="1">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>20</v>
@@ -1137,15 +1144,15 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="63" customHeight="1">
+    <row r="13" spans="1:11" ht="67.5" customHeight="1">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1156,15 +1163,15 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="58.5" customHeight="1">
+    <row r="14" spans="1:11" ht="63" customHeight="1">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1175,15 +1182,15 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="87" customHeight="1">
+    <row r="15" spans="1:11" ht="58.5" customHeight="1">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1194,15 +1201,15 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="99" customHeight="1">
+    <row r="16" spans="1:11" ht="87" customHeight="1">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1213,15 +1220,15 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="76.5" customHeight="1">
+    <row r="17" spans="1:11" ht="99" customHeight="1">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1232,15 +1239,15 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="89.25" customHeight="1">
+    <row r="18" spans="1:11" ht="76.5" customHeight="1">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1251,15 +1258,15 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="47.25" customHeight="1">
+    <row r="19" spans="1:11" ht="89.25" customHeight="1">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1270,12 +1277,12 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="39.75" customHeight="1">
+    <row r="20" spans="1:11" ht="47.25" customHeight="1">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>33</v>
@@ -1289,11 +1296,18 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+    <row r="21" spans="1:11" ht="39.75" customHeight="1">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1306,7 +1320,6 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -2328,12 +2341,18 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" ht="15" customHeight="1">
+    <row r="101" spans="1:11" ht="15.75" customHeight="1">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
     </row>
     <row r="102" spans="1:11" ht="15" customHeight="1">
       <c r="A102" s="2"/>
@@ -2356,6 +2375,13 @@
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
     </row>
+    <row r="105" spans="1:11" ht="15" customHeight="1">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>